<commit_message>
Commit done on 23 may
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelFiles/LoginData.xlsx
+++ b/src/main/resources/ExcelFiles/LoginData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="40" windowWidth="19100" windowHeight="7300"/>
+    <workbookView xWindow="80" yWindow="40" windowWidth="19100" windowHeight="7300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DPdata" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Password</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>ghhg</t>
+  </si>
+  <si>
+    <t>jhj</t>
   </si>
 </sst>
 </file>
@@ -364,8 +370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -405,12 +411,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>